<commit_message>
Changes to tap custom playsheets and reports to reflect changes in TAP databases from DHMSM to MHS Genesis and for Disposition property changes
git-svn-id: svn://107.170.10.188:8080/Semoss/dev@14571 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 9e3df22f19c7f987e3f645f714cab0f16af293e8
</commit_message>
<xml_diff>
--- a/export/Reports/FactSheets/System_Disposition_Fact_Sheet_Template.xlsx
+++ b/export/Reports/FactSheets/System_Disposition_Fact_Sheet_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkirk\workspace\SEMOSS\export\Reports\FactSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace\Semoss\export\Reports\FactSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" tabRatio="873" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" tabRatio="873"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -96,6 +96,7 @@
     <definedName name="xz">[10]Data!$B$3:$B$12</definedName>
   </definedNames>
   <calcPr calcId="152511" calcOnSave="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -249,12 +250,6 @@
     <t># of interfaces to develop</t>
   </si>
   <si>
-    <t># of data objects to receive from DHMSM</t>
-  </si>
-  <si>
-    <t># of data objects provided to DHMSM</t>
-  </si>
-  <si>
     <t>Facility Command (Army, Navy, AF, Joint)</t>
   </si>
   <si>
@@ -403,12 +398,6 @@
     <t>System Disposition</t>
   </si>
   <si>
-    <t>% of data created that DHMSM will provide</t>
-  </si>
-  <si>
-    <t>% of business logic that DHMSM will provide</t>
-  </si>
-  <si>
     <t>Requirements from Requirements Traceability Matrix</t>
   </si>
   <si>
@@ -425,10 +414,6 @@
   </si>
   <si>
     <t>This section defines the current interfaces for @SYSTEM@ that will continue to be supported as the system is transitioned to the future-state environment.</t>
-  </si>
-  <si>
-    <t>Budget information, when available, is broken out by the type of appropriation: Procurement (OP), Operations and Maintenance (O&amp;M), and Research, Development, Test, and Evaluation (RDT&amp;E).
-This report breaks out the required transition costs to migrate @SYSTEM@ to the future-state environment for those systems that will not be replaced by the new electronic health record. The transition modernization estimates are broken into three categories: (1) interface modernization costs, which address the investment requried to modernize the interfaces in order to support data exchange between @SYSTEM@ and the DHMSM EHR; (2) hardware and software modernization costs required to ensure that technical support for @SYSTEM@ is available; and (3) DIACAP costs required to maintain the IA posture of @SYSTEM@.</t>
   </si>
   <si>
     <r>
@@ -462,6 +447,22 @@
   </si>
   <si>
     <t># of Interfaces Supported</t>
+  </si>
+  <si>
+    <t>% of data created that MHS GENESIS will provide</t>
+  </si>
+  <si>
+    <t>% of business logic that MHS GENESIS will provide</t>
+  </si>
+  <si>
+    <t># of data objects provided to MHS GENESIS</t>
+  </si>
+  <si>
+    <t># of data objects to receive from MHS GENESIS</t>
+  </si>
+  <si>
+    <t>Budget information, when available, is broken out by the type of appropriation: Procurement (OP), Operations and Maintenance (O&amp;M), and Research, Development, Test, and Evaluation (RDT&amp;E).
+This report breaks out the required transition costs to migrate @SYSTEM@ to the future-state environment for those systems that will not be replaced by the new electronic health record. The transition modernization estimates are broken into three categories: (1) interface modernization costs, which address the investment requried to modernize the interfaces in order to support data exchange between @SYSTEM@ and MHS GENESIS; (2) hardware and software modernization costs required to ensure that technical support for @SYSTEM@ is available; and (3) DIACAP costs required to maintain the IA posture of @SYSTEM@.</t>
   </si>
 </sst>
 </file>
@@ -25261,32 +25262,32 @@
   </sheetPr>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A15" zoomScale="90" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:K17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16:S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.109375" customWidth="1"/>
     <col min="2" max="2" width="8" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="10" customWidth="1"/>
     <col min="4" max="4" width="8" style="10" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
     <col min="7" max="7" width="9" style="10" customWidth="1"/>
-    <col min="8" max="9" width="7.5703125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="10" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="1.28515625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="4.7109375" style="10" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="10" customWidth="1"/>
+    <col min="8" max="9" width="7.5546875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="1.88671875" style="10" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="1.33203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" style="10" customWidth="1"/>
     <col min="16" max="16" width="8" style="10" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="10" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="1.140625" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="10"/>
+    <col min="19" max="19" width="13.6640625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="1.109375" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1" ht="100.5" customHeight="1">
@@ -25296,7 +25297,7 @@
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="73" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E1" s="73"/>
       <c r="F1" s="73"/>
@@ -25337,11 +25338,11 @@
     </row>
     <row r="3" spans="1:20" ht="23.25" customHeight="1">
       <c r="B3" s="77" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" s="77"/>
       <c r="D3" s="80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E3" s="81"/>
       <c r="F3" s="81"/>
@@ -25361,11 +25362,11 @@
     </row>
     <row r="4" spans="1:20" ht="25.5" customHeight="1">
       <c r="B4" s="77" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" s="77"/>
       <c r="D4" s="78" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E4" s="79"/>
       <c r="F4" s="79"/>
@@ -25464,7 +25465,7 @@
     <row r="8" spans="1:20" s="15" customFormat="1" ht="21" customHeight="1">
       <c r="A8"/>
       <c r="B8" s="113" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C8" s="113"/>
       <c r="D8" s="113"/>
@@ -25488,7 +25489,7 @@
     <row r="9" spans="1:20" s="15" customFormat="1" ht="33.75" customHeight="1">
       <c r="A9"/>
       <c r="B9" s="138" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C9" s="138"/>
       <c r="D9" s="138"/>
@@ -25512,12 +25513,12 @@
     <row r="10" spans="1:20" s="15" customFormat="1" ht="99" customHeight="1">
       <c r="A10"/>
       <c r="B10" s="103" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C10" s="103"/>
       <c r="D10" s="103"/>
       <c r="E10" s="140" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F10" s="141"/>
       <c r="G10" s="141"/>
@@ -25538,7 +25539,7 @@
     <row r="11" spans="1:20" s="15" customFormat="1" ht="36" customHeight="1">
       <c r="A11"/>
       <c r="B11" s="91" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C11" s="92"/>
       <c r="D11" s="92"/>
@@ -25551,7 +25552,7 @@
       <c r="I11" s="89"/>
       <c r="J11" s="89"/>
       <c r="K11" s="91" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="L11" s="92"/>
       <c r="M11" s="92"/>
@@ -25640,7 +25641,7 @@
     <row r="15" spans="1:20" s="15" customFormat="1" ht="62.25" customHeight="1">
       <c r="A15"/>
       <c r="B15" s="136" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C15" s="137"/>
       <c r="D15" s="136" t="s">
@@ -25665,17 +25666,17 @@
       </c>
       <c r="N15" s="137"/>
       <c r="O15" s="64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P15" s="136" t="s">
         <v>48</v>
       </c>
       <c r="Q15" s="137"/>
       <c r="R15" s="64" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="S15" s="65" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="T15"/>
     </row>
@@ -25714,11 +25715,11 @@
       </c>
       <c r="Q16" s="121"/>
       <c r="R16" s="118">
-        <f>COUNTIF('Future Interface Development'!B7:B500,"DHMSM")</f>
+        <f>COUNTIF('Future Interface Development'!B7:B500,"MHS GENESIS")</f>
         <v>0</v>
       </c>
       <c r="S16" s="118">
-        <f>COUNTIF('Future Interface Development'!A7:A500,"DHMSM")</f>
+        <f>COUNTIF('Future Interface Development'!A7:A500,"MHS GENESIS")</f>
         <v>0</v>
       </c>
       <c r="T16"/>
@@ -26262,14 +26263,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="7" width="13.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="7" width="13.109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -26282,9 +26283,9 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="143" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="143"/>
       <c r="C2" s="143"/>
@@ -26306,11 +26307,11 @@
     </row>
     <row r="4" spans="1:8" ht="32.25" customHeight="1">
       <c r="A4" s="144" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="145"/>
       <c r="C4" s="146" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" s="146"/>
       <c r="E4" s="146"/>
@@ -26328,33 +26329,33 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="D6" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="E6" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="F6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="G6" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="H6" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="68" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:8" ht="13.8">
       <c r="A7" s="69"/>
       <c r="B7" s="69"/>
       <c r="C7" s="69"/>
@@ -26390,11 +26391,11 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="7" width="13.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="7" width="13.109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -26407,9 +26408,9 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="143" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" s="143"/>
       <c r="C2" s="143"/>
@@ -26431,11 +26432,11 @@
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
       <c r="A4" s="144" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="145"/>
       <c r="C4" s="146" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D4" s="146"/>
       <c r="E4" s="146"/>
@@ -26453,33 +26454,33 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="D6" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="E6" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="F6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="G6" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="H6" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="68" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:8" ht="13.8">
       <c r="A7" s="69"/>
       <c r="B7" s="69"/>
       <c r="C7" s="69"/>
@@ -26515,10 +26516,10 @@
       <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="7" width="13.140625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="7" width="13.109375" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -26530,9 +26531,9 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75">
+    <row r="2" spans="1:7" ht="18">
       <c r="A2" s="143" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="143"/>
       <c r="C2" s="143"/>
@@ -26552,11 +26553,11 @@
     </row>
     <row r="4" spans="1:7" ht="36.75" customHeight="1">
       <c r="A4" s="144" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="145"/>
       <c r="C4" s="146" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" s="146"/>
       <c r="E4" s="146"/>
@@ -26572,30 +26573,30 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="28.8">
       <c r="A6" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="D6" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="E6" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="F6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="G6" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="68" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:7" ht="13.8">
       <c r="A7" s="69"/>
       <c r="B7" s="69"/>
       <c r="C7" s="69"/>
@@ -26626,17 +26627,17 @@
   </sheetPr>
   <dimension ref="A1:K535"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="7" customWidth="1"/>
-    <col min="3" max="4" width="12.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="7" customWidth="1"/>
+    <col min="3" max="4" width="12.88671875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -26683,7 +26684,7 @@
     <row r="4" spans="1:11" ht="36.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="66" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="148" t="s">
         <v>26</v>
@@ -26710,7 +26711,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75">
+    <row r="6" spans="1:11" ht="15.6">
       <c r="A6" s="2"/>
       <c r="B6" s="156" t="s">
         <v>13</v>
@@ -26730,7 +26731,7 @@
       <c r="C7" s="154"/>
       <c r="D7" s="154"/>
       <c r="E7" s="61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -30464,14 +30465,14 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="B5" sqref="B5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="1.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="1" customWidth="1"/>
   </cols>
@@ -30491,7 +30492,7 @@
     <row r="2" spans="1:10" ht="21">
       <c r="A2" s="1"/>
       <c r="B2" s="155" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C2" s="155"/>
       <c r="D2" s="155"/>
@@ -30502,14 +30503,14 @@
       <c r="I2" s="155"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:10" ht="18">
+    <row r="3" spans="1:10" ht="17.399999999999999">
       <c r="A3" s="1"/>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="180" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="181"/>
       <c r="D4" s="181"/>
@@ -30523,7 +30524,7 @@
     <row r="5" spans="1:10" ht="125.25" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="157" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C5" s="157"/>
       <c r="D5" s="157"/>
@@ -30541,7 +30542,7 @@
     <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="173" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="174"/>
       <c r="D7" s="174"/>
@@ -30552,7 +30553,7 @@
       <c r="I7" s="175"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75">
+    <row r="8" spans="1:10" ht="15.6">
       <c r="B8" s="176" t="s">
         <v>18</v>
       </c>
@@ -30648,7 +30649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+    <row r="12" spans="1:10" ht="15" thickBot="1">
       <c r="B12" s="182" t="s">
         <v>17</v>
       </c>
@@ -30678,7 +30679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="15" thickBot="1">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -30687,9 +30688,9 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+    <row r="14" spans="1:10" ht="15" thickBot="1">
       <c r="B14" s="184" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="185"/>
       <c r="D14" s="185"/>
@@ -30701,26 +30702,26 @@
     </row>
     <row r="15" spans="1:10" ht="20.25" customHeight="1" thickBot="1">
       <c r="B15" s="159" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="160"/>
       <c r="D15" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="G15" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="H15" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="I15" s="54" t="s">
         <v>70</v>
-      </c>
-      <c r="H15" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="54" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -30728,7 +30729,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" s="26">
         <v>0</v>
@@ -30753,7 +30754,7 @@
     <row r="17" spans="2:9">
       <c r="B17" s="187"/>
       <c r="C17" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" s="31">
         <v>0</v>
@@ -30778,7 +30779,7 @@
     <row r="18" spans="2:9">
       <c r="B18" s="187"/>
       <c r="C18" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" s="31">
         <v>0</v>
@@ -30803,7 +30804,7 @@
     <row r="19" spans="2:9">
       <c r="B19" s="187"/>
       <c r="C19" s="30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="31">
         <v>0</v>
@@ -30828,7 +30829,7 @@
     <row r="20" spans="2:9">
       <c r="B20" s="187"/>
       <c r="C20" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D20" s="31">
         <v>0</v>
@@ -30853,7 +30854,7 @@
     <row r="21" spans="2:9">
       <c r="B21" s="187"/>
       <c r="C21" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" s="32">
         <v>0</v>
@@ -30878,7 +30879,7 @@
     <row r="22" spans="2:9">
       <c r="B22" s="188"/>
       <c r="C22" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="32">
         <v>0</v>
@@ -30900,9 +30901,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15.75" thickBot="1">
+    <row r="23" spans="2:9" ht="15" thickBot="1">
       <c r="B23" s="161" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="162"/>
       <c r="D23" s="35">
@@ -30930,12 +30931,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickTop="1">
+    <row r="24" spans="2:9" ht="15" thickTop="1">
       <c r="B24" s="189" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="26">
         <v>0</v>
@@ -30960,7 +30961,7 @@
     <row r="25" spans="2:9">
       <c r="B25" s="187"/>
       <c r="C25" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D25" s="31">
         <v>0</v>
@@ -30985,7 +30986,7 @@
     <row r="26" spans="2:9">
       <c r="B26" s="187"/>
       <c r="C26" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="31">
         <v>0</v>
@@ -31010,7 +31011,7 @@
     <row r="27" spans="2:9">
       <c r="B27" s="187"/>
       <c r="C27" s="30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="31">
         <v>0</v>
@@ -31035,7 +31036,7 @@
     <row r="28" spans="2:9">
       <c r="B28" s="187"/>
       <c r="C28" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="31">
         <v>0</v>
@@ -31060,7 +31061,7 @@
     <row r="29" spans="2:9">
       <c r="B29" s="187"/>
       <c r="C29" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="32">
         <v>0</v>
@@ -31085,7 +31086,7 @@
     <row r="30" spans="2:9">
       <c r="B30" s="188"/>
       <c r="C30" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D30" s="32">
         <v>0</v>
@@ -31101,7 +31102,7 @@
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="163" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="164"/>
       <c r="D31" s="38">
@@ -31131,7 +31132,7 @@
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="169" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" s="170"/>
       <c r="D32" s="48"/>
@@ -31143,7 +31144,7 @@
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="171" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="172"/>
       <c r="D33" s="41">
@@ -31168,7 +31169,7 @@
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="169" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" s="170"/>
       <c r="D34" s="48"/>
@@ -31178,9 +31179,9 @@
       <c r="H34" s="49"/>
       <c r="I34" s="50"/>
     </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1">
+    <row r="35" spans="2:9" ht="15" thickBot="1">
       <c r="B35" s="167" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" s="168"/>
       <c r="D35" s="41">
@@ -31203,9 +31204,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="15.75" thickBot="1">
+    <row r="36" spans="2:9" ht="15" thickBot="1">
       <c r="B36" s="165" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" s="166"/>
       <c r="D36" s="44">
@@ -31273,12 +31274,12 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="14.4">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>9</v>
@@ -31292,7 +31293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="14.4">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -31317,7 +31318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="14.4">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -31342,7 +31343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="14.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -31367,7 +31368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="14.4">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -31392,7 +31393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" ht="14.4">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -31417,7 +31418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="14.4">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -31437,7 +31438,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="B8" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -31474,12 +31475,12 @@
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -31487,7 +31488,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -31495,7 +31496,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -31517,20 +31518,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="59" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="14.88671875" style="59" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="58" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="59" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="60">
         <v>0.18</v>
@@ -31538,7 +31539,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="60">
         <v>0.15</v>
@@ -31546,7 +31547,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="59" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" s="60">
         <v>1.7999999999999999E-2</v>

</xml_diff>